<commit_message>
Updated pjm5bus.xlsx GENCLS Sn to make vf in range.
</commit_message>
<xml_diff>
--- a/andes/cases/5bus/pjm5bus.xlsx
+++ b/andes/cases/5bus/pjm5bus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/notebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82325B0-3C87-B64E-8B23-8B61510B6690}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABE592D-4562-7740-83D3-EAC8D7541971}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="23080" windowHeight="13000" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24960" yWindow="1680" windowWidth="28840" windowHeight="21660" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -679,7 +679,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2062,9 +2062,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2145,7 +2145,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H2">
         <v>230</v>
@@ -2198,7 +2198,7 @@
         <v>2</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="H3">
         <v>230</v>
@@ -2251,7 +2251,7 @@
         <v>3</v>
       </c>
       <c r="G4">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H4">
         <v>230</v>
@@ -2304,7 +2304,7 @@
         <v>4</v>
       </c>
       <c r="G5">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="H5">
         <v>230</v>
@@ -2349,7 +2349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>

</xml_diff>

<commit_message>
Updated text for InitChecker.
</commit_message>
<xml_diff>
--- a/andes/cases/5bus/pjm5bus.xlsx
+++ b/andes/cases/5bus/pjm5bus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABE592D-4562-7740-83D3-EAC8D7541971}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8874204-9F01-DD4A-942A-B091A22492AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24960" yWindow="1680" windowWidth="28840" windowHeight="21660" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2064,7 +2064,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Changed GENCLS.xq to GENCLS.xd1. xq is now an `ExtService`.
</commit_message>
<xml_diff>
--- a/andes/cases/5bus/pjm5bus.xlsx
+++ b/andes/cases/5bus/pjm5bus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8874204-9F01-DD4A-942A-B091A22492AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2D7437-0879-1A43-9C3E-1E8B2FE6823C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24960" yWindow="1680" windowWidth="28840" windowHeight="21660" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -222,9 +222,6 @@
     <t>xl</t>
   </si>
   <si>
-    <t>xq</t>
-  </si>
-  <si>
     <t>kp</t>
   </si>
   <si>
@@ -274,6 +271,9 @@
   </si>
   <si>
     <t>Line</t>
+  </si>
+  <si>
+    <t>xd1</t>
   </si>
 </sst>
 </file>
@@ -2064,7 +2064,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2110,22 +2110,22 @@
         <v>63</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -2370,10 +2370,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>27</v>
@@ -2382,22 +2382,22 @@
         <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -2594,13 +2594,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2614,7 +2614,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F2">
         <v>6</v>

</xml_diff>